<commit_message>
modicada la lista de tareas
</commit_message>
<xml_diff>
--- a/organizacion/ListaDeTareas.xlsx
+++ b/organizacion/ListaDeTareas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19320" windowHeight="7995" activeTab="1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>Tareas</t>
   </si>
@@ -176,9 +176,6 @@
     <t>1 hora</t>
   </si>
   <si>
-    <t>i) cambiar nombre en la parte superios</t>
-  </si>
-  <si>
     <t>ver DIAGRAMA DE ESTADO con MODELO DE DOMINIO</t>
   </si>
   <si>
@@ -285,13 +282,34 @@
   </si>
   <si>
     <t>falta actualizarlo segun nuevos casos de uso y verificar si estan completos</t>
+  </si>
+  <si>
+    <t>i) cambiar nombre en la parte superior</t>
+  </si>
+  <si>
+    <t>referencias</t>
+  </si>
+  <si>
+    <t>ver al final (jueves o viernes)</t>
+  </si>
+  <si>
+    <t>en accion</t>
+  </si>
+  <si>
+    <t>para revisar</t>
+  </si>
+  <si>
+    <t>hecho</t>
+  </si>
+  <si>
+    <t>pendiente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,24 +348,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -361,6 +361,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,28 +410,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +526,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -538,7 +560,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -714,14 +735,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.140625" bestFit="1" customWidth="1"/>
@@ -730,194 +751,194 @@
     <col min="5" max="5" width="75.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="3" spans="1:5">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="12"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="12"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="7"/>
+      <c r="B12" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="12"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="12"/>
-      <c r="B12" s="14" t="s">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="7"/>
+      <c r="B13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="12"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="12"/>
-      <c r="B13" s="14" t="s">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="7"/>
+      <c r="B14" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="12"/>
-      <c r="B14" s="14" t="s">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="7"/>
+      <c r="B15" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="12"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12"/>
-      <c r="B15" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="12"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -925,14 +946,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.5703125" customWidth="1"/>
@@ -942,231 +963,234 @@
     <col min="8" max="8" width="32.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="5" t="s">
+      <c r="E1" s="15"/>
+      <c r="F1" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="5"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:8">
+      <c r="A3" s="17">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="18">
         <v>0</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="4" spans="1:8">
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="E4" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="4"/>
-      <c r="H4" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="17" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:8">
+      <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="G5" s="4">
-        <v>0</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
+    <row r="6" spans="1:8">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="5">
         <v>1</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:8">
+      <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F7" t="s">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:8">
+      <c r="A8" s="11">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="12">
         <v>0.75</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:8">
+      <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="C10" t="s">
         <v>62</v>
       </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="H9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="E10" t="s">
         <v>63</v>
-      </c>
-      <c r="E10" t="s">
-        <v>64</v>
       </c>
       <c r="F10" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="1">
         <v>0.4</v>
       </c>
       <c r="H10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1185,14 +1209,14 @@
       <c r="F11" t="s">
         <v>46</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="1">
         <v>0.33</v>
       </c>
       <c r="H11" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="C12" t="s">
         <v>50</v>
       </c>
@@ -1200,119 +1224,157 @@
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
         <v>46</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="1">
         <v>0.15</v>
       </c>
       <c r="H12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:8">
+      <c r="A13" s="17">
         <v>8</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="17"/>
+      <c r="F13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="13">
+        <v>9</v>
+      </c>
+      <c r="B14" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D13" t="s">
+      <c r="C14" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" t="s">
-        <v>59</v>
-      </c>
-      <c r="G14" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="H14" t="s">
+      <c r="E14" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
+    <row r="15" spans="1:8">
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="4">
+        <v>1</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="C17" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="5">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="H17" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E17" t="s">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="F17" t="s">
-        <v>29</v>
-      </c>
-      <c r="G17" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="F18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="5">
+        <v>1</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" t="s">
-        <v>85</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
-      </c>
-      <c r="G18" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="H18" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G19" s="4"/>
+    <row r="19" spans="1:8">
+      <c r="G19" s="1"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>95</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>